<commit_message>
Added updated documents to delivrables
</commit_message>
<xml_diff>
--- a/Deliverables/DanielSohler_ProductionResources.xlsx
+++ b/Deliverables/DanielSohler_ProductionResources.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myaie-my.sharepoint.com/personal/s192126_students_aie_edu_au/Documents/Year 2 Work/Designing for Clients/Deliverables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s192126\Documents\GitHub\Vizard_Repo\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="504" documentId="11_F25DC773A252ABDACC1048E7099C679C5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51702B7B-AE67-40A4-806C-6D5E9EC538D4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7E151D-F4EA-412C-BE55-605F4A9FFBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="110">
   <si>
     <t>Weeks</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Very High</t>
   </si>
   <si>
-    <t>Null</t>
-  </si>
-  <si>
     <t>Pixel art, used to frame game view</t>
   </si>
   <si>
@@ -169,12 +166,6 @@
     <t>Prototyping</t>
   </si>
   <si>
-    <t>Modelling</t>
-  </si>
-  <si>
-    <t>UI/Art Creation</t>
-  </si>
-  <si>
     <t>Audio</t>
   </si>
   <si>
@@ -223,15 +214,6 @@
     <t>Needs to fit in spell slot, and in inventory screen</t>
   </si>
   <si>
-    <t>Enemy Health Bar/UI_Enemey_Healthbar_Foregournd</t>
-  </si>
-  <si>
-    <t>Enemy Health Bar/UI_Enemey_Healthbar_Fill</t>
-  </si>
-  <si>
-    <t>Enemy Health Bar/UI_Enemey_Healthbar_Background</t>
-  </si>
-  <si>
     <t>Enemy, UI</t>
   </si>
   <si>
@@ -275,13 +257,112 @@
   </si>
   <si>
     <t>Tick Icon/UI_Tick_Icon</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>Texturing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setting up project </t>
+  </si>
+  <si>
+    <t>Setting up movement, and verb system</t>
+  </si>
+  <si>
+    <t>Verb system combination system</t>
+  </si>
+  <si>
+    <t>Animating</t>
+  </si>
+  <si>
+    <t>Getting verbs added</t>
+  </si>
+  <si>
+    <t>1st pass UI Sprites</t>
+  </si>
+  <si>
+    <t>2nd pass UI sprites</t>
+  </si>
+  <si>
+    <t>1st pass VFX sprites</t>
+  </si>
+  <si>
+    <t>2nd pass VFX sprites</t>
+  </si>
+  <si>
+    <t>Start scroll texture</t>
+  </si>
+  <si>
+    <t>Start envrionment textures</t>
+  </si>
+  <si>
+    <t>Animate chests and doors</t>
+  </si>
+  <si>
+    <t>Animate enemies</t>
+  </si>
+  <si>
+    <t>Tidy Up spell effects</t>
+  </si>
+  <si>
+    <t>Enemy attack system</t>
+  </si>
+  <si>
+    <t>Enemy Health Bar/UI_Enemy_Healthbar_Foregournd</t>
+  </si>
+  <si>
+    <t>Enemy Health Bar/UI_Enemy_Healthbar_Fill</t>
+  </si>
+  <si>
+    <t>Enemy Health Bar/UI_Enemy_Healthbar_Background</t>
+  </si>
+  <si>
+    <t>VFX</t>
+  </si>
+  <si>
+    <t>Visual Feedback</t>
+  </si>
+  <si>
+    <t>Looks like red spark of fire</t>
+  </si>
+  <si>
+    <t>Looks like blue spark of electricity</t>
+  </si>
+  <si>
+    <t>Looks like sickly green light</t>
+  </si>
+  <si>
+    <t>For when Green verbs are used in spells</t>
+  </si>
+  <si>
+    <t>For when Blue verbs are used in spells</t>
+  </si>
+  <si>
+    <t>For when Red verbs are used in spells</t>
+  </si>
+  <si>
+    <t>Red Verb FX/FX_Red_Verb</t>
+  </si>
+  <si>
+    <t>Blue Verb FX/FX_Blue_Verb</t>
+  </si>
+  <si>
+    <t>Green Verb FX/FX_Green_Verb</t>
+  </si>
+  <si>
+    <t>Making menus to enter/exit game</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,8 +422,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -385,6 +480,16 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -564,10 +669,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -618,6 +725,31 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -663,9 +795,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -701,13 +834,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>57151</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2114550</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>1526676</xdr:rowOff>
@@ -745,15 +878,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>307268</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2095500</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>1530480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -789,15 +922,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1905000</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -833,15 +966,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>381001</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2057400</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>1314450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -877,16 +1010,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>400051</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2076451</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>16999</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>17000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -921,16 +1054,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1825149</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>4083</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>4082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -959,6 +1092,309 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>217716</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1387930</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>92008</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C34941-E95E-434B-8BDA-472E0FFD6EFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10300609" y="7062107"/>
+          <a:ext cx="1170214" cy="1166972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1253097</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1088573</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="Powerful electrical discharge, lightning strike impact place realistic -  Nohat - Free for designer">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7245C49-FD1C-44A3-AFA3-5F26961EF432}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10246179" y="5932715"/>
+          <a:ext cx="1089811" cy="1088572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1183821</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1058038</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12" descr="Spark | Pixel Art Maker">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFA0D1E0-20CF-403F-B216-FB18CD202134}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10082894" y="4830538"/>
+          <a:ext cx="1183820" cy="1058036"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>231322</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1226671</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>993323</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14" descr="Editing pause button 2 - Free online pixel art drawing tool - Pixilart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE65AA33-69EB-40B9-A58D-3430C86BA531}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10314215" y="8137072"/>
+          <a:ext cx="995349" cy="993322"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>81642</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1333499</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1234405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16" descr="Pixel Art Green Check Mark Stock Vector (Royalty Free) 1072643492 |  Shutterstock">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0134794-DD38-485E-B5D0-09C5D5D48CE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect b="7912"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10164535" y="9212037"/>
+          <a:ext cx="1251857" cy="1234404"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1229,101 +1665,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF16"/>
+  <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="7" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="22" t="s">
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="28" t="s">
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="24"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="33"/>
     </row>
     <row r="2" spans="1:32" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="25"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="26"/>
-      <c r="AF2" s="27"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="34"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="36"/>
     </row>
     <row r="3" spans="1:32" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -1427,18 +1865,20 @@
       <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
+      <c r="B4" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
@@ -1460,21 +1900,29 @@
       <c r="AF4" s="12"/>
     </row>
     <row r="5" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
+      <c r="A5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
@@ -1495,24 +1943,30 @@
     </row>
     <row r="6" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
+        <v>48</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
       <c r="T6" s="12"/>
@@ -1531,15 +1985,18 @@
     </row>
     <row r="7" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
+        <v>79</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="28"/>
+      <c r="E7" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="24"/>
+      <c r="H7" s="20"/>
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
@@ -1549,13 +2006,13 @@
       <c r="O7" s="20"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="20"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="20"/>
       <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
       <c r="AA7" s="12"/>
@@ -1567,14 +2024,22 @@
     </row>
     <row r="8" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="20"/>
+        <v>77</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
@@ -1592,7 +2057,7 @@
       <c r="V8" s="20"/>
       <c r="W8" s="20"/>
       <c r="X8" s="20"/>
-      <c r="Y8" s="12"/>
+      <c r="Y8" s="20"/>
       <c r="Z8" s="12"/>
       <c r="AA8" s="12"/>
       <c r="AB8" s="12"/>
@@ -1603,14 +2068,18 @@
     </row>
     <row r="9" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
+        <v>83</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
@@ -1639,50 +2108,50 @@
     </row>
     <row r="10" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
+        <v>78</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
       <c r="T10" s="20"/>
       <c r="U10" s="20"/>
       <c r="V10" s="20"/>
       <c r="W10" s="20"/>
       <c r="X10" s="20"/>
       <c r="Y10" s="20"/>
-      <c r="Z10" s="20"/>
-      <c r="AA10" s="20"/>
-      <c r="AB10" s="20"/>
-      <c r="AC10" s="20"/>
-      <c r="AD10" s="20"/>
-      <c r="AE10" s="21"/>
-      <c r="AF10" s="21"/>
-    </row>
-    <row r="11" spans="1:32" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z10" s="12"/>
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="12"/>
+      <c r="AE10" s="12"/>
+      <c r="AF10" s="12"/>
+    </row>
+    <row r="11" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
@@ -1706,22 +2175,58 @@
       <c r="AB11" s="20"/>
       <c r="AC11" s="20"/>
       <c r="AD11" s="20"/>
-      <c r="AE11" s="20"/>
-      <c r="AF11" s="20"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="D14" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" ht="30" x14ac:dyDescent="0.25">
-      <c r="D15" s="13" t="s">
-        <v>53</v>
+      <c r="AE11" s="21"/>
+      <c r="AF11" s="21"/>
+    </row>
+    <row r="12" spans="1:32" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="20"/>
+      <c r="AD12" s="20"/>
+      <c r="AE12" s="20"/>
+      <c r="AF12" s="20"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="D15" s="12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:32" ht="30" x14ac:dyDescent="0.25">
-      <c r="D16" s="14" t="s">
-        <v>54</v>
+      <c r="D16" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D17" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1733,8 +2238,8 @@
     <mergeCell ref="R1:V2"/>
     <mergeCell ref="W1:AA2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:AF11">
-    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
+  <conditionalFormatting sqref="B4:AF12">
+    <cfRule type="duplicateValues" dxfId="0" priority="9"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1743,10 +2248,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B41D32D-E896-44BD-9C12-C6C4EE434494}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,34 +2259,34 @@
     <col min="1" max="1" width="54.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="32.5703125" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" customWidth="1"/>
-    <col min="8" max="8" width="35.28515625" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="36"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="45"/>
     </row>
     <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -1794,19 +2299,19 @@
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
@@ -1820,22 +2325,22 @@
         <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="29" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>13</v>
@@ -1844,456 +2349,517 @@
         <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="1"/>
+      <c r="H6" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" ht="171" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="F13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="D14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="30"/>
+    </row>
+    <row r="17" spans="1:8" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="F17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="30"/>
+    </row>
+    <row r="18" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="5" t="s">
+      <c r="C18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="5" t="s">
+      <c r="E19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="G19" s="1"/>
+      <c r="H19" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="5" t="s">
+      <c r="F20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="30"/>
     </row>
     <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="1"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="1"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="1"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="1"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="1"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="1"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="1"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="1"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="4"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="1"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="4"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="1"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="1"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="2"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>